<commit_message>
feat:done laporan formulir 11
</commit_message>
<xml_diff>
--- a/public/assets/report/report-11.xlsx
+++ b/public/assets/report/report-11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laravel\sistem-pelaporan-terpadu-puskesmas\public\assets\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A3CD56-F354-43EF-B0D3-66408BD0A984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949C730D-19E2-4F5D-8A1D-DD2B93E52550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C168CAB2-6B48-4071-981D-C5105527579B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="538">
   <si>
     <t>FORMULIR 11</t>
   </si>
@@ -1554,9 +1554,6 @@
     <t>Perdarahan post partum</t>
   </si>
   <si>
-    <t>072.1</t>
-  </si>
-  <si>
     <t>Persalinan lama</t>
   </si>
   <si>
@@ -1638,13 +1635,10 @@
     <t>NIP. 199803042022032013</t>
   </si>
   <si>
-    <t>MARET</t>
-  </si>
-  <si>
-    <t>Makassar, 5 April 2025</t>
-  </si>
-  <si>
     <t>K35.9</t>
+  </si>
+  <si>
+    <t>O72.1</t>
   </si>
 </sst>
 </file>
@@ -2362,8 +2356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEB7FF2-217F-486D-963B-5ACFB82FB8D4}">
   <dimension ref="A1:S364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A348" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P357" sqref="P357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2475,9 +2469,7 @@
       <c r="J5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>537</v>
-      </c>
+      <c r="K5" s="7"/>
       <c r="L5" s="1"/>
       <c r="M5" s="5" t="s">
         <v>4</v>
@@ -2529,9 +2521,7 @@
       <c r="J7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="8">
-        <v>2025</v>
-      </c>
+      <c r="K7" s="8"/>
       <c r="L7" s="1"/>
       <c r="M7" s="5" t="s">
         <v>9</v>
@@ -3928,7 +3918,7 @@
         <v>87</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="D51" s="28"/>
       <c r="E51" s="28"/>
@@ -13157,7 +13147,7 @@
         <v>508</v>
       </c>
       <c r="C342" s="13" t="s">
-        <v>509</v>
+        <v>537</v>
       </c>
       <c r="D342" s="26"/>
       <c r="E342" s="26"/>
@@ -13181,10 +13171,10 @@
         <v>12</v>
       </c>
       <c r="B343" s="13" t="s">
+        <v>509</v>
+      </c>
+      <c r="C343" s="13" t="s">
         <v>510</v>
-      </c>
-      <c r="C343" s="13" t="s">
-        <v>511</v>
       </c>
       <c r="D343" s="26"/>
       <c r="E343" s="26"/>
@@ -13208,10 +13198,10 @@
         <v>13</v>
       </c>
       <c r="B344" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="C344" s="13" t="s">
         <v>512</v>
-      </c>
-      <c r="C344" s="13" t="s">
-        <v>513</v>
       </c>
       <c r="D344" s="26"/>
       <c r="E344" s="26"/>
@@ -13235,10 +13225,10 @@
         <v>14</v>
       </c>
       <c r="B345" s="13" t="s">
+        <v>513</v>
+      </c>
+      <c r="C345" s="13" t="s">
         <v>514</v>
-      </c>
-      <c r="C345" s="13" t="s">
-        <v>515</v>
       </c>
       <c r="D345" s="29"/>
       <c r="E345" s="26"/>
@@ -13262,10 +13252,10 @@
         <v>15</v>
       </c>
       <c r="B346" s="13" t="s">
+        <v>515</v>
+      </c>
+      <c r="C346" s="13" t="s">
         <v>516</v>
-      </c>
-      <c r="C346" s="13" t="s">
-        <v>517</v>
       </c>
       <c r="D346" s="18"/>
       <c r="E346" s="18"/>
@@ -13286,10 +13276,10 @@
     </row>
     <row r="347" spans="1:19" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A347" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="B347" s="13" t="s">
         <v>518</v>
-      </c>
-      <c r="B347" s="13" t="s">
-        <v>519</v>
       </c>
       <c r="C347" s="14"/>
       <c r="D347" s="27"/>
@@ -13314,10 +13304,10 @@
         <v>1</v>
       </c>
       <c r="B348" s="13" t="s">
+        <v>519</v>
+      </c>
+      <c r="C348" s="13" t="s">
         <v>520</v>
-      </c>
-      <c r="C348" s="13" t="s">
-        <v>521</v>
       </c>
       <c r="D348" s="28"/>
       <c r="E348" s="28"/>
@@ -13341,10 +13331,10 @@
         <v>2</v>
       </c>
       <c r="B349" s="13" t="s">
+        <v>521</v>
+      </c>
+      <c r="C349" s="13" t="s">
         <v>522</v>
-      </c>
-      <c r="C349" s="13" t="s">
-        <v>523</v>
       </c>
       <c r="D349" s="8"/>
       <c r="E349" s="8"/>
@@ -13507,10 +13497,10 @@
         <v>3</v>
       </c>
       <c r="B353" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="C353" s="13" t="s">
         <v>524</v>
-      </c>
-      <c r="C353" s="13" t="s">
-        <v>525</v>
       </c>
       <c r="D353" s="29"/>
       <c r="E353" s="26"/>
@@ -13534,10 +13524,10 @@
         <v>4</v>
       </c>
       <c r="B354" s="13" t="s">
+        <v>525</v>
+      </c>
+      <c r="C354" s="13" t="s">
         <v>526</v>
-      </c>
-      <c r="C354" s="13" t="s">
-        <v>527</v>
       </c>
       <c r="D354" s="18"/>
       <c r="E354" s="18"/>
@@ -13561,10 +13551,10 @@
         <v>5</v>
       </c>
       <c r="B355" s="13" t="s">
+        <v>527</v>
+      </c>
+      <c r="C355" s="13" t="s">
         <v>528</v>
-      </c>
-      <c r="C355" s="13" t="s">
-        <v>529</v>
       </c>
       <c r="D355" s="28"/>
       <c r="E355" s="28"/>
@@ -13620,9 +13610,7 @@
       <c r="M357" s="1"/>
       <c r="N357" s="1"/>
       <c r="O357" s="1"/>
-      <c r="P357" s="24" t="s">
-        <v>538</v>
-      </c>
+      <c r="P357" s="24"/>
       <c r="Q357" s="1"/>
       <c r="R357" s="1"/>
       <c r="S357" s="1"/>
@@ -13630,7 +13618,7 @@
     <row r="358" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A358" s="1"/>
       <c r="B358" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C358" s="1"/>
       <c r="D358" s="1"/>
@@ -13653,7 +13641,7 @@
     <row r="359" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A359" s="1"/>
       <c r="B359" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C359" s="1"/>
       <c r="D359" s="1"/>
@@ -13669,7 +13657,7 @@
       <c r="N359" s="1"/>
       <c r="O359" s="1"/>
       <c r="P359" s="24" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Q359" s="1"/>
       <c r="R359" s="2"/>
@@ -13741,7 +13729,7 @@
     <row r="363" spans="1:19" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A363" s="1"/>
       <c r="B363" s="25" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C363" s="1"/>
       <c r="D363" s="1"/>
@@ -13757,7 +13745,7 @@
       <c r="N363" s="1"/>
       <c r="O363" s="1"/>
       <c r="P363" s="24" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="Q363" s="1"/>
       <c r="R363" s="1"/>
@@ -13766,7 +13754,7 @@
     <row r="364" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A364" s="1"/>
       <c r="B364" s="25" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C364" s="1"/>
       <c r="D364" s="1"/>
@@ -13782,7 +13770,7 @@
       <c r="N364" s="1"/>
       <c r="O364" s="1"/>
       <c r="P364" s="24" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="Q364" s="1"/>
       <c r="R364" s="1"/>

</xml_diff>